<commit_message>
EPBDS-10604 Support Java 15
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/ITEST/itest.HttpStatuses/openl-repository/deployments/http-statuses-test/MAIN.xlsx
+++ b/ITEST/itest.HttpStatuses/openl-repository/deployments/http-statuses-test/MAIN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openl-pub\ITEST\itest.HttpStatuses\openl-repository\deployments\http-statuses-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\ITEST\itest.HttpStatuses\openl-repository\deployments\http-statuses-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C772E457-BC78-439B-8302-8060EFF85ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="8190"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Method void throwUserException()</t>
   </si>
@@ -71,19 +72,22 @@
     <t>Method void throwNPE()</t>
   </si>
   <si>
-    <t>Integer.decode(null);</t>
-  </si>
-  <si>
     <t>Method Integer throwNFE()</t>
   </si>
   <si>
     <t>return Integer.decode("");</t>
+  </si>
+  <si>
+    <t>java.util.Objects.requireNonNull(arg);</t>
+  </si>
+  <si>
+    <t>Object arg = null;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -155,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -171,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -211,7 +215,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -246,6 +250,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -281,9 +302,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,10 +494,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -525,22 +563,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -549,7 +592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -587,7 +630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B6:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>